<commit_message>
Deliver the first stage
</commit_message>
<xml_diff>
--- a/crop_names.xlsx
+++ b/crop_names.xlsx
@@ -387,9 +387,6 @@
     <t>Conifer trees</t>
   </si>
   <si>
-    <t>Deciduous orchard</t>
-  </si>
-  <si>
     <t>- Apples</t>
   </si>
   <si>
@@ -412,6 +409,9 @@
   </si>
   <si>
     <t>Olives</t>
+  </si>
+  <si>
+    <t>m. Deciduous orchard</t>
   </si>
 </sst>
 </file>
@@ -864,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1384,48 +1384,48 @@
       </c>
     </row>
     <row r="108" spans="1:1" ht="15" thickBot="1">
-      <c r="A108" s="2" t="s">
-        <v>102</v>
+      <c r="A108" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15" thickBot="1">
       <c r="A109" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15" thickBot="1">
       <c r="A110" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15" thickBot="1">
       <c r="A111" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15" thickBot="1">
       <c r="A112" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15" thickBot="1">
       <c r="A113" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15" thickBot="1">
       <c r="A114" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15" thickBot="1">
       <c r="A115" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15" thickBot="1">
       <c r="A116" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1433,6 +1433,7 @@
     <hyperlink ref="A57" location="_bookmark6" display="_bookmark6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>